<commit_message>
assign color transition to percent funding
</commit_message>
<xml_diff>
--- a/CrowdfundingBook.xlsx
+++ b/CrowdfundingBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yslav\Desktop\MonashBootcamp\challenge-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398D0D75-30D3-4685-AA04-1DE0E2E38A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1EE886-9EC6-4001-A86C-19FEF5872EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="735" windowWidth="33195" windowHeight="19995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43680" yWindow="735" windowWidth="22785" windowHeight="19995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crowdfunding" sheetId="1" r:id="rId1"/>
@@ -7015,8 +7015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A961" workbookViewId="0">
-      <selection activeCell="F1003" sqref="F1003"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -55079,25 +55079,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="canceled">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="canceled">
       <formula>NOT(ISERROR(SEARCH("canceled",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="live">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="live">
       <formula>NOT(ISERROR(SEARCH("live",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="live">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="live">
       <formula>NOT(ISERROR(SEARCH("live",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="successful">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="successful">
       <formula>NOT(ISERROR(SEARCH("successful",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="failed">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="failed">
       <formula>NOT(ISERROR(SEARCH("failed",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="live">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="live">
       <formula>NOT(ISERROR(SEARCH("live",I11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="100"/>
+        <cfvo type="num" val="200"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FF0070C0"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
hide buttons on pivot charts
</commit_message>
<xml_diff>
--- a/CrowdfundingBook.xlsx
+++ b/CrowdfundingBook.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yslav\Desktop\MonashBootcamp\challenge-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B6D1D6-0C67-486C-8280-6F9C7DE8650E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D670AE94-8A87-4A14-B744-D6F9A02E83B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43680" yWindow="735" windowWidth="28410" windowHeight="19995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43680" yWindow="735" windowWidth="25635" windowHeight="19995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Per Category" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Per Sub-Category" sheetId="3" r:id="rId2"/>
     <sheet name="Crowdfunding" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -7696,7 +7696,6 @@
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
         <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
@@ -7722,7 +7721,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[CrowdfundingBook.xlsx]Sheet2!PivotTable2</c:name>
+    <c:name>[CrowdfundingBook.xlsx]Per Sub-Category!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -7968,7 +7967,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$4:$B$5</c:f>
+              <c:f>'Per Sub-Category'!$B$4:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7989,7 +7988,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$6:$A$30</c:f>
+              <c:f>'Per Sub-Category'!$A$6:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
@@ -8069,7 +8068,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$6:$B$30</c:f>
+              <c:f>'Per Sub-Category'!$B$6:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -8132,7 +8131,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$4:$C$5</c:f>
+              <c:f>'Per Sub-Category'!$C$4:$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8153,7 +8152,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$6:$A$30</c:f>
+              <c:f>'Per Sub-Category'!$A$6:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
@@ -8233,7 +8232,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$6:$C$30</c:f>
+              <c:f>'Per Sub-Category'!$C$6:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -8317,7 +8316,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$4:$D$5</c:f>
+              <c:f>'Per Sub-Category'!$D$4:$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8338,7 +8337,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$6:$A$30</c:f>
+              <c:f>'Per Sub-Category'!$A$6:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
@@ -8418,7 +8417,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$6:$D$30</c:f>
+              <c:f>'Per Sub-Category'!$D$6:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -8469,7 +8468,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$4:$E$5</c:f>
+              <c:f>'Per Sub-Category'!$E$4:$E$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8494,7 +8493,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$6:$A$30</c:f>
+              <c:f>'Per Sub-Category'!$A$6:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
@@ -8574,7 +8573,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$E$6:$E$30</c:f>
+              <c:f>'Per Sub-Category'!$E$6:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -8866,7 +8865,6 @@
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
         <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
@@ -30351,7 +30349,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B6ECA70C-146A-4847-AD38-EAE27943C2CC}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B6ECA70C-146A-4847-AD38-EAE27943C2CC}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A4:F30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -30901,8 +30899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C5258C-8993-4593-B1DC-2320FEAF0A21}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -31181,8 +31179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03CD45F-F9FE-4DDD-8011-F2143266C2F6}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>